<commit_message>
Update net check-in list
</commit_message>
<xml_diff>
--- a/SARES-net-check-in.xlsx
+++ b/SARES-net-check-in.xlsx
@@ -1,12 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\srben\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3404C12B-B8D6-4294-AB04-A244E2782AAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="1695" yWindow="1230" windowWidth="16545" windowHeight="9870" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -475,9 +497,6 @@
     <t>KWW</t>
   </si>
   <si>
-    <t>Roster updated 02/04/2023</t>
-  </si>
-  <si>
     <t>Erez</t>
   </si>
   <si>
@@ -509,77 +528,84 @@
   </si>
   <si>
     <t>MZM</t>
+  </si>
+  <si>
+    <t>Roster updated 03/28/2023</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yy"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
-    <font/>
     <font>
-      <sz val="12.0"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <u/>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FF0563C1"/>
       <name val="Arial"/>
     </font>
@@ -589,7 +615,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -665,41 +691,39 @@
     </fill>
   </fills>
   <borders count="10">
-    <border/>
     <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -709,11 +733,31 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="medium">
@@ -728,17 +772,20 @@
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="medium">
         <color rgb="FF000000"/>
       </left>
+      <right/>
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -747,259 +794,146 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="65">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
-    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="1" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="6" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="3" fillId="0" fontId="6" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="4" fillId="4" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="5" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="5" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="4" fillId="2" fontId="8" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left" readingOrder="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="6" fillId="5" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="3" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="3" fillId="2" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="3" fillId="6" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="7" fillId="5" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="4" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="4" fillId="2" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="4" fillId="6" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="4" fillId="2" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="8" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="9" fillId="2" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="9" fillId="6" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="9" fillId="2" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="7" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="3" fillId="7" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="9" fillId="2" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="4" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="4" fillId="8" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="4" fillId="2" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="3" fillId="2" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="4" fillId="8" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="9" fillId="2" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="4" fillId="9" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="4" fillId="9" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="9" fillId="9" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="4" fillId="10" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="4" fillId="10" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="9" fillId="10" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="4" fillId="11" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="4" fillId="11" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="9" fillId="11" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="12" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="4" fillId="5" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="4" fillId="5" fontId="8" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="4" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="4" fillId="6" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="12" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="12" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="12" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="12" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="10" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="4" fillId="12" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="3" fillId="2" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="4" fillId="2" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="4" fillId="2" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="4" fillId="13" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="8" fillId="13" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -1189,34 +1123,39 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
+  <dimension ref="A1:P61"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="L33" sqref="L33"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="6.0"/>
-    <col customWidth="1" min="3" max="3" width="6.25"/>
-    <col customWidth="1" min="4" max="4" width="6.38"/>
-    <col customWidth="1" min="5" max="5" width="6.0"/>
-    <col customWidth="1" min="6" max="6" width="7.13"/>
-    <col customWidth="1" min="7" max="7" width="13.5"/>
-    <col customWidth="1" min="8" max="8" width="7.13"/>
-    <col customWidth="1" min="9" max="9" width="6.13"/>
-    <col customWidth="1" min="10" max="10" width="6.0"/>
-    <col customWidth="1" min="11" max="11" width="3.5"/>
-    <col customWidth="1" min="14" max="14" width="5.63"/>
+    <col min="1" max="1" width="6" customWidth="1"/>
+    <col min="3" max="3" width="6.28515625" customWidth="1"/>
+    <col min="4" max="4" width="6.42578125" customWidth="1"/>
+    <col min="5" max="5" width="6" customWidth="1"/>
+    <col min="6" max="6" width="7.140625" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" customWidth="1"/>
+    <col min="8" max="8" width="7.140625" customWidth="1"/>
+    <col min="9" max="9" width="6.140625" customWidth="1"/>
+    <col min="10" max="10" width="6" customWidth="1"/>
+    <col min="11" max="11" width="3.42578125" customWidth="1"/>
+    <col min="14" max="14" width="5.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="1"/>
@@ -1228,675 +1167,686 @@
       <c r="I1" s="5"/>
       <c r="J1" s="1"/>
     </row>
-    <row r="2">
+    <row r="2" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
       <c r="B2" s="7"/>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="12"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="60"/>
+      <c r="G2" s="61"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="9"/>
       <c r="J2" s="6"/>
-      <c r="L2" s="13" t="s">
+      <c r="L2" s="10" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="14"/>
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
-      <c r="J3" s="19"/>
-      <c r="L3" s="20"/>
-    </row>
-    <row r="4">
-      <c r="A4" s="21" t="s">
+    <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="11"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="15"/>
+      <c r="L3" s="16"/>
+    </row>
+    <row r="4" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="23" t="s">
+      <c r="C4" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="24" t="s">
+      <c r="D4" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="25"/>
-      <c r="F4" s="26" t="s">
+      <c r="E4" s="21"/>
+      <c r="F4" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="27" t="s">
+      <c r="G4" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="28" t="s">
+      <c r="H4" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="29" t="s">
+      <c r="I4" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="J4" s="30"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="15"/>
-      <c r="B5" s="31" t="s">
+      <c r="J4" s="26"/>
+    </row>
+    <row r="5" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="11"/>
+      <c r="B5" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="32" t="s">
+      <c r="C5" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="33" t="s">
+      <c r="D5" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="34"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="27" t="s">
+      <c r="E5" s="30"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="28" t="s">
+      <c r="H5" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="29" t="s">
+      <c r="I5" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="30"/>
-      <c r="K5" s="35"/>
-      <c r="L5" s="36" t="s">
+      <c r="J5" s="26"/>
+      <c r="K5" s="15"/>
+      <c r="L5" s="62" t="s">
         <v>16</v>
       </c>
-      <c r="M5" s="10"/>
-      <c r="N5" s="37"/>
-    </row>
-    <row r="6">
-      <c r="A6" s="15"/>
-      <c r="B6" s="31" t="s">
+      <c r="M5" s="61"/>
+      <c r="N5" s="31"/>
+    </row>
+    <row r="6" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="11"/>
+      <c r="B6" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="32" t="s">
+      <c r="C6" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="33" t="s">
+      <c r="D6" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="38"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="27" t="s">
+      <c r="E6" s="30"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="H6" s="28" t="s">
+      <c r="H6" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="I6" s="29" t="s">
+      <c r="I6" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="J6" s="30"/>
-      <c r="K6" s="35"/>
-      <c r="L6" s="28" t="s">
+      <c r="J6" s="26"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="M6" s="39"/>
-      <c r="N6" s="40"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="15"/>
-      <c r="B7" s="31" t="s">
+      <c r="M6" s="23"/>
+      <c r="N6" s="32"/>
+    </row>
+    <row r="7" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="11"/>
+      <c r="B7" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="32" t="s">
+      <c r="C7" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="33" t="s">
+      <c r="D7" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="E7" s="38"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="27" t="s">
+      <c r="E7" s="30"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="H7" s="28" t="s">
+      <c r="H7" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="I7" s="29" t="s">
+      <c r="I7" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="J7" s="30"/>
-      <c r="K7" s="35"/>
-      <c r="L7" s="28" t="s">
+      <c r="J7" s="26"/>
+      <c r="K7" s="15"/>
+      <c r="L7" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="M7" s="39"/>
-      <c r="N7" s="40"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="15"/>
-      <c r="B8" s="31" t="s">
+      <c r="M7" s="23"/>
+      <c r="N7" s="32"/>
+    </row>
+    <row r="8" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="11"/>
+      <c r="B8" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="32" t="s">
+      <c r="C8" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="33" t="s">
+      <c r="D8" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="E8" s="34"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="31" t="s">
+      <c r="E8" s="30"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="H8" s="32" t="s">
+      <c r="H8" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="I8" s="29" t="s">
+      <c r="I8" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="J8" s="30"/>
-      <c r="K8" s="35"/>
-      <c r="L8" s="28" t="s">
+      <c r="J8" s="26"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="M8" s="39"/>
-      <c r="N8" s="40"/>
-    </row>
-    <row r="9">
-      <c r="A9" s="15"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="31" t="s">
+      <c r="M8" s="23"/>
+      <c r="N8" s="32"/>
+    </row>
+    <row r="9" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="H9" s="32" t="s">
+      <c r="H9" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="I9" s="29" t="s">
+      <c r="I9" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="J9" s="41"/>
-      <c r="K9" s="35"/>
-      <c r="L9" s="28" t="s">
+      <c r="J9" s="26"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="M9" s="39"/>
-      <c r="N9" s="40"/>
-    </row>
-    <row r="10">
-      <c r="A10" s="21" t="s">
+      <c r="M9" s="23"/>
+      <c r="N9" s="32"/>
+    </row>
+    <row r="10" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="B10" s="22" t="s">
+      <c r="B10" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="C10" s="23" t="s">
+      <c r="C10" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="24" t="s">
+      <c r="D10" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="E10" s="42"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="31" t="s">
+      <c r="E10" s="33"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="H10" s="32" t="s">
+      <c r="H10" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="I10" s="29" t="s">
+      <c r="I10" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="J10" s="41"/>
-      <c r="K10" s="35"/>
-      <c r="L10" s="28" t="s">
+      <c r="J10" s="26"/>
+      <c r="K10" s="15"/>
+      <c r="L10" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="M10" s="39"/>
-      <c r="N10" s="40"/>
-    </row>
-    <row r="11">
-      <c r="B11" s="31" t="s">
+      <c r="M10" s="23"/>
+      <c r="N10" s="32"/>
+    </row>
+    <row r="11" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="C11" s="32" t="s">
+      <c r="C11" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="D11" s="33" t="s">
+      <c r="D11" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="E11" s="38"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="31" t="s">
+      <c r="E11" s="30"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="H11" s="32" t="s">
+      <c r="H11" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="I11" s="29" t="s">
+      <c r="I11" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="J11" s="41"/>
-      <c r="K11" s="35"/>
-      <c r="L11" s="28" t="s">
+      <c r="J11" s="26"/>
+      <c r="K11" s="15"/>
+      <c r="L11" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="M11" s="39"/>
-      <c r="N11" s="43">
+      <c r="M11" s="23"/>
+      <c r="N11" s="34">
         <f>J35</f>
         <v>0</v>
       </c>
     </row>
-    <row r="12">
-      <c r="B12" s="31" t="s">
+    <row r="12" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="C12" s="32" t="s">
+      <c r="C12" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="D12" s="33" t="s">
+      <c r="D12" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="E12" s="38"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="31" t="s">
+      <c r="E12" s="30"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="H12" s="32" t="s">
+      <c r="H12" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="I12" s="29" t="s">
+      <c r="I12" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="J12" s="41"/>
-      <c r="K12" s="35"/>
-      <c r="L12" s="28" t="s">
+      <c r="J12" s="26"/>
+      <c r="K12" s="15"/>
+      <c r="L12" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="M12" s="39"/>
-      <c r="N12" s="40"/>
-    </row>
-    <row r="13">
-      <c r="B13" s="31" t="s">
+      <c r="M12" s="23"/>
+      <c r="N12" s="32"/>
+    </row>
+    <row r="13" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="C13" s="32" t="s">
+      <c r="C13" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="33" t="s">
+      <c r="D13" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="E13" s="34"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="31" t="s">
+      <c r="E13" s="30"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="27" t="s">
         <v>62</v>
       </c>
-      <c r="H13" s="32" t="s">
+      <c r="H13" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="I13" s="29" t="s">
+      <c r="I13" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="J13" s="41"/>
-      <c r="K13" s="35"/>
-      <c r="L13" s="28" t="s">
+      <c r="J13" s="26"/>
+      <c r="K13" s="15"/>
+      <c r="L13" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="M13" s="39"/>
-      <c r="N13" s="40"/>
-    </row>
-    <row r="14">
-      <c r="A14" s="15"/>
-      <c r="B14" s="31" t="s">
+      <c r="M13" s="23"/>
+      <c r="N13" s="32"/>
+    </row>
+    <row r="14" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="11"/>
+      <c r="B14" s="27" t="s">
         <v>66</v>
       </c>
-      <c r="C14" s="32" t="s">
+      <c r="C14" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="D14" s="33" t="s">
+      <c r="D14" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="E14" s="34"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="31" t="s">
+      <c r="E14" s="30"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="H14" s="32" t="s">
+      <c r="H14" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="I14" s="29" t="s">
+      <c r="I14" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="J14" s="30"/>
-      <c r="K14" s="35"/>
-      <c r="L14" s="39"/>
-      <c r="M14" s="39"/>
-      <c r="N14" s="44"/>
-    </row>
-    <row r="15">
-      <c r="B15" s="31" t="s">
+      <c r="J14" s="26"/>
+      <c r="K14" s="15"/>
+      <c r="L14" s="23"/>
+      <c r="M14" s="23"/>
+      <c r="N14" s="28"/>
+    </row>
+    <row r="15" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="C15" s="32" t="s">
+      <c r="C15" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="D15" s="33" t="s">
+      <c r="D15" s="29" t="s">
         <v>73</v>
       </c>
-      <c r="E15" s="38"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="31" t="s">
+      <c r="E15" s="30"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="27" t="s">
         <v>74</v>
       </c>
-      <c r="H15" s="32" t="s">
+      <c r="H15" s="28" t="s">
         <v>75</v>
       </c>
-      <c r="I15" s="29" t="s">
+      <c r="I15" s="25" t="s">
         <v>76</v>
       </c>
-      <c r="J15" s="30"/>
-      <c r="K15" s="35"/>
-      <c r="L15" s="45" t="s">
+      <c r="J15" s="26"/>
+      <c r="K15" s="15"/>
+      <c r="L15" s="35" t="s">
         <v>77</v>
       </c>
-      <c r="M15" s="46"/>
-      <c r="N15" s="47"/>
-    </row>
-    <row r="16">
-      <c r="A16" s="11"/>
-      <c r="B16" s="31" t="s">
+      <c r="M15" s="36"/>
+      <c r="N15" s="37">
+        <f>SUM(N6:N13)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="8"/>
+      <c r="B16" s="27" t="s">
         <v>78</v>
       </c>
-      <c r="C16" s="32" t="s">
+      <c r="C16" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="D16" s="33" t="s">
+      <c r="D16" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="E16" s="38"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="31" t="s">
+      <c r="E16" s="30"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="27" t="s">
         <v>80</v>
       </c>
-      <c r="H16" s="32" t="s">
+      <c r="H16" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="I16" s="29" t="s">
+      <c r="I16" s="25" t="s">
         <v>81</v>
       </c>
-      <c r="J16" s="30"/>
-      <c r="K16" s="12"/>
-      <c r="L16" s="48" t="s">
+      <c r="J16" s="26"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="38" t="s">
         <v>82</v>
       </c>
-      <c r="M16" s="49"/>
-      <c r="N16" s="50"/>
-    </row>
-    <row r="17">
-      <c r="A17" s="15"/>
-      <c r="B17" s="31" t="s">
+      <c r="M16" s="39"/>
+      <c r="N16" s="40"/>
+    </row>
+    <row r="17" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="11"/>
+      <c r="B17" s="27" t="s">
         <v>83</v>
       </c>
-      <c r="C17" s="32" t="s">
+      <c r="C17" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="D17" s="33" t="s">
+      <c r="D17" s="29" t="s">
         <v>84</v>
       </c>
-      <c r="E17" s="34"/>
-      <c r="F17" s="15"/>
-      <c r="G17" s="31" t="s">
+      <c r="E17" s="30"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="27" t="s">
         <v>85</v>
       </c>
-      <c r="H17" s="32" t="s">
+      <c r="H17" s="28" t="s">
         <v>86</v>
       </c>
-      <c r="I17" s="29" t="s">
+      <c r="I17" s="25" t="s">
         <v>87</v>
       </c>
-      <c r="J17" s="30"/>
-      <c r="L17" s="51" t="s">
+      <c r="J17" s="26"/>
+      <c r="L17" s="41" t="s">
         <v>88</v>
       </c>
-      <c r="M17" s="52"/>
-      <c r="N17" s="53"/>
-    </row>
-    <row r="18">
-      <c r="A18" s="15"/>
-      <c r="B18" s="31" t="s">
+      <c r="M17" s="42"/>
+      <c r="N17" s="43"/>
+    </row>
+    <row r="18" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="11"/>
+      <c r="B18" s="27" t="s">
         <v>89</v>
       </c>
-      <c r="C18" s="32" t="s">
+      <c r="C18" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="D18" s="33" t="s">
+      <c r="D18" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="E18" s="38"/>
-      <c r="F18" s="54"/>
-      <c r="G18" s="31" t="s">
+      <c r="E18" s="30"/>
+      <c r="F18" s="44"/>
+      <c r="G18" s="27" t="s">
         <v>91</v>
       </c>
-      <c r="H18" s="32" t="s">
+      <c r="H18" s="28" t="s">
         <v>92</v>
       </c>
-      <c r="I18" s="29" t="s">
+      <c r="I18" s="25" t="s">
         <v>93</v>
       </c>
-      <c r="J18" s="41"/>
-      <c r="K18" s="35"/>
-      <c r="L18" s="55" t="s">
+      <c r="J18" s="26"/>
+      <c r="K18" s="15"/>
+      <c r="L18" s="45" t="s">
         <v>94</v>
       </c>
-      <c r="M18" s="56"/>
-      <c r="N18" s="56">
+      <c r="M18" s="45"/>
+      <c r="N18" s="45">
         <f>SUM(N15:N17)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="19">
-      <c r="A19" s="15"/>
-      <c r="B19" s="31" t="s">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A19" s="11"/>
+      <c r="B19" s="27" t="s">
         <v>95</v>
       </c>
-      <c r="C19" s="32" t="s">
+      <c r="C19" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="D19" s="33" t="s">
+      <c r="D19" s="29" t="s">
         <v>96</v>
       </c>
-      <c r="E19" s="38"/>
-      <c r="G19" s="57" t="s">
+      <c r="E19" s="30"/>
+      <c r="G19" s="46" t="s">
         <v>97</v>
       </c>
-      <c r="H19" s="58" t="s">
+      <c r="H19" s="47" t="s">
         <v>98</v>
       </c>
-      <c r="I19" s="59" t="s">
+      <c r="I19" s="48" t="s">
         <v>99</v>
       </c>
-      <c r="J19" s="58"/>
-      <c r="K19" s="35"/>
-    </row>
-    <row r="20">
-      <c r="A20" s="15"/>
-      <c r="B20" s="57" t="s">
+      <c r="J19" s="47"/>
+      <c r="K19" s="15"/>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A20" s="11"/>
+      <c r="B20" s="46" t="s">
         <v>100</v>
       </c>
-      <c r="C20" s="58" t="s">
+      <c r="C20" s="47" t="s">
         <v>101</v>
       </c>
-      <c r="D20" s="59" t="s">
+      <c r="D20" s="48" t="s">
         <v>102</v>
       </c>
-      <c r="E20" s="58"/>
-      <c r="G20" s="60"/>
-      <c r="H20" s="61"/>
-      <c r="I20" s="62"/>
-      <c r="J20" s="63"/>
-      <c r="K20" s="35"/>
-    </row>
-    <row r="21">
-      <c r="A21" s="15"/>
-      <c r="B21" s="57" t="s">
+      <c r="E20" s="47"/>
+      <c r="G20" s="49"/>
+      <c r="H20" s="50"/>
+      <c r="I20" s="51"/>
+      <c r="J20" s="52"/>
+      <c r="K20" s="15"/>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A21" s="11"/>
+      <c r="B21" s="46" t="s">
         <v>103</v>
       </c>
-      <c r="C21" s="58" t="s">
+      <c r="C21" s="47" t="s">
         <v>37</v>
       </c>
-      <c r="D21" s="59" t="s">
+      <c r="D21" s="48" t="s">
         <v>102</v>
       </c>
-      <c r="E21" s="64"/>
-      <c r="F21" s="21" t="s">
+      <c r="E21" s="46"/>
+      <c r="F21" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="G21" s="27" t="s">
+      <c r="G21" s="23" t="s">
         <v>105</v>
       </c>
-      <c r="H21" s="23" t="s">
+      <c r="H21" s="19" t="s">
         <v>106</v>
       </c>
-      <c r="I21" s="24" t="s">
+      <c r="I21" s="20" t="s">
         <v>107</v>
       </c>
-      <c r="J21" s="65"/>
-      <c r="K21" s="35"/>
-      <c r="L21" s="66" t="s">
+      <c r="J21" s="53"/>
+      <c r="K21" s="15"/>
+      <c r="L21" s="63" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="15"/>
-      <c r="F22" s="15"/>
-      <c r="G22" s="31" t="s">
+      <c r="M21" s="64"/>
+      <c r="N21" s="64"/>
+      <c r="O21" s="64"/>
+      <c r="P21" s="64"/>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A22" s="11"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="27" t="s">
         <v>109</v>
       </c>
-      <c r="H22" s="32" t="s">
+      <c r="H22" s="28" t="s">
         <v>110</v>
       </c>
-      <c r="I22" s="33" t="s">
+      <c r="I22" s="29" t="s">
         <v>111</v>
       </c>
-      <c r="J22" s="34"/>
-      <c r="K22" s="66"/>
-      <c r="L22" s="67" t="s">
+      <c r="J22" s="30"/>
+      <c r="K22" s="6"/>
+      <c r="L22" s="8" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="23">
-      <c r="A23" s="21" t="s">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A23" s="17" t="s">
         <v>113</v>
       </c>
-      <c r="B23" s="22" t="s">
+      <c r="B23" s="18" t="s">
         <v>114</v>
       </c>
-      <c r="C23" s="23" t="s">
+      <c r="C23" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="D23" s="24" t="s">
+      <c r="D23" s="20" t="s">
         <v>115</v>
       </c>
-      <c r="E23" s="68"/>
-      <c r="G23" s="31" t="s">
+      <c r="E23" s="33"/>
+      <c r="G23" s="27" t="s">
         <v>116</v>
       </c>
-      <c r="H23" s="32" t="s">
+      <c r="H23" s="28" t="s">
         <v>117</v>
       </c>
-      <c r="I23" s="33" t="s">
+      <c r="I23" s="29" t="s">
         <v>118</v>
       </c>
-      <c r="J23" s="38"/>
-      <c r="K23" s="66"/>
-      <c r="L23" s="66" t="s">
+      <c r="J23" s="30"/>
+      <c r="K23" s="6"/>
+      <c r="L23" s="63" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="24">
-      <c r="B24" s="31" t="s">
+      <c r="M23" s="64"/>
+      <c r="N23" s="64"/>
+      <c r="O23" s="64"/>
+      <c r="P23" s="64"/>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B24" s="27" t="s">
         <v>120</v>
       </c>
-      <c r="C24" s="32" t="s">
+      <c r="C24" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="D24" s="33" t="s">
+      <c r="D24" s="29" t="s">
         <v>121</v>
       </c>
-      <c r="E24" s="38"/>
-      <c r="G24" s="31" t="s">
+      <c r="E24" s="30"/>
+      <c r="G24" s="27" t="s">
         <v>85</v>
       </c>
-      <c r="H24" s="32" t="s">
+      <c r="H24" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="I24" s="33" t="s">
+      <c r="I24" s="29" t="s">
         <v>122</v>
       </c>
-      <c r="J24" s="34"/>
-      <c r="K24" s="69"/>
-      <c r="L24" s="70" t="s">
+      <c r="J24" s="30"/>
+      <c r="K24" s="54"/>
+      <c r="L24" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="M24" s="69"/>
-      <c r="N24" s="69"/>
-      <c r="O24" s="69"/>
+      <c r="M24" s="54"/>
+      <c r="N24" s="54"/>
+      <c r="O24" s="54"/>
       <c r="P24" s="6"/>
     </row>
-    <row r="25">
-      <c r="B25" s="31" t="s">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B25" s="27" t="s">
         <v>124</v>
       </c>
-      <c r="C25" s="32" t="s">
+      <c r="C25" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="D25" s="33" t="s">
+      <c r="D25" s="29" t="s">
         <v>125</v>
       </c>
-      <c r="E25" s="34"/>
-      <c r="G25" s="31" t="s">
+      <c r="E25" s="30"/>
+      <c r="G25" s="27" t="s">
         <v>126</v>
       </c>
-      <c r="H25" s="32" t="s">
+      <c r="H25" s="28" t="s">
         <v>86</v>
       </c>
-      <c r="I25" s="33" t="s">
+      <c r="I25" s="29" t="s">
         <v>127</v>
       </c>
-      <c r="J25" s="34"/>
-      <c r="K25" s="69"/>
-      <c r="L25" s="69"/>
-      <c r="M25" s="69"/>
-      <c r="N25" s="69"/>
-      <c r="O25" s="69"/>
+      <c r="J25" s="30"/>
+      <c r="K25" s="54"/>
+      <c r="L25" s="54"/>
+      <c r="M25" s="54"/>
+      <c r="N25" s="54"/>
+      <c r="O25" s="54"/>
       <c r="P25" s="6"/>
     </row>
-    <row r="26">
-      <c r="B26" s="31" t="s">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B26" s="27" t="s">
         <v>128</v>
       </c>
-      <c r="C26" s="32" t="s">
+      <c r="C26" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="D26" s="33" t="s">
+      <c r="D26" s="29" t="s">
         <v>129</v>
       </c>
-      <c r="E26" s="38"/>
-      <c r="G26" s="31" t="s">
+      <c r="E26" s="30"/>
+      <c r="G26" s="27" t="s">
         <v>126</v>
       </c>
-      <c r="H26" s="32" t="s">
+      <c r="H26" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="I26" s="33" t="s">
+      <c r="I26" s="29" t="s">
         <v>130</v>
       </c>
-      <c r="J26" s="34"/>
-      <c r="K26" s="71"/>
-      <c r="L26" s="66" t="s">
+      <c r="J26" s="30"/>
+      <c r="K26" s="55"/>
+      <c r="L26" s="6" t="s">
         <v>131</v>
       </c>
       <c r="M26" s="6"/>
@@ -1904,30 +1854,30 @@
       <c r="O26" s="6"/>
       <c r="P26" s="6"/>
     </row>
-    <row r="27">
-      <c r="A27" s="14"/>
-      <c r="B27" s="31" t="s">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A27" s="11"/>
+      <c r="B27" s="27" t="s">
         <v>132</v>
       </c>
-      <c r="C27" s="32" t="s">
+      <c r="C27" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="D27" s="33" t="s">
+      <c r="D27" s="29" t="s">
         <v>133</v>
       </c>
-      <c r="E27" s="34"/>
-      <c r="G27" s="31" t="s">
+      <c r="E27" s="30"/>
+      <c r="G27" s="27" t="s">
         <v>134</v>
       </c>
-      <c r="H27" s="32" t="s">
+      <c r="H27" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="I27" s="33" t="s">
+      <c r="I27" s="29" t="s">
         <v>135</v>
       </c>
-      <c r="J27" s="34"/>
-      <c r="K27" s="71"/>
-      <c r="L27" s="72" t="s">
+      <c r="J27" s="30"/>
+      <c r="K27" s="55"/>
+      <c r="L27" s="6" t="s">
         <v>136</v>
       </c>
       <c r="M27" s="6"/>
@@ -1935,345 +1885,348 @@
       <c r="O27" s="6"/>
       <c r="P27" s="6"/>
     </row>
-    <row r="28">
-      <c r="B28" s="31" t="s">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B28" s="27" t="s">
         <v>137</v>
       </c>
-      <c r="C28" s="32" t="s">
+      <c r="C28" s="28" t="s">
         <v>138</v>
       </c>
-      <c r="D28" s="33" t="s">
+      <c r="D28" s="29" t="s">
         <v>139</v>
       </c>
-      <c r="E28" s="34"/>
-      <c r="F28" s="15"/>
-      <c r="G28" s="31" t="s">
+      <c r="E28" s="30"/>
+      <c r="F28" s="11"/>
+      <c r="G28" s="27" t="s">
         <v>140</v>
       </c>
-      <c r="H28" s="32" t="s">
+      <c r="H28" s="28" t="s">
         <v>141</v>
       </c>
-      <c r="I28" s="33" t="s">
+      <c r="I28" s="29" t="s">
         <v>142</v>
       </c>
-      <c r="J28" s="38"/>
-      <c r="K28" s="66"/>
-      <c r="N28" s="66"/>
+      <c r="J28" s="30"/>
+      <c r="K28" s="6"/>
+      <c r="N28" s="6"/>
       <c r="O28" s="6"/>
       <c r="P28" s="6"/>
     </row>
-    <row r="29">
-      <c r="A29" s="11"/>
-      <c r="B29" s="31" t="s">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A29" s="8"/>
+      <c r="B29" s="27" t="s">
         <v>143</v>
       </c>
-      <c r="C29" s="32" t="s">
+      <c r="C29" s="28" t="s">
         <v>144</v>
       </c>
-      <c r="D29" s="33" t="s">
+      <c r="D29" s="29" t="s">
         <v>145</v>
       </c>
-      <c r="E29" s="38"/>
-      <c r="G29" s="31" t="s">
+      <c r="E29" s="30"/>
+      <c r="G29" s="27" t="s">
         <v>137</v>
       </c>
-      <c r="H29" s="32" t="s">
+      <c r="H29" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="I29" s="33" t="s">
+      <c r="I29" s="29" t="s">
         <v>146</v>
       </c>
-      <c r="J29" s="34"/>
-    </row>
-    <row r="30">
-      <c r="A30" s="15"/>
-      <c r="B30" s="31" t="s">
+      <c r="J29" s="30"/>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A30" s="11"/>
+      <c r="B30" s="27" t="s">
         <v>147</v>
       </c>
-      <c r="C30" s="32" t="s">
+      <c r="C30" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="D30" s="33" t="s">
+      <c r="D30" s="29" t="s">
         <v>148</v>
       </c>
-      <c r="E30" s="38"/>
-    </row>
-    <row r="31">
-      <c r="A31" s="15"/>
-      <c r="B31" s="31" t="s">
+      <c r="E30" s="30"/>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A31" s="11"/>
+      <c r="B31" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="C31" s="32" t="s">
+      <c r="C31" s="28" t="s">
         <v>75</v>
       </c>
-      <c r="D31" s="33" t="s">
+      <c r="D31" s="29" t="s">
         <v>149</v>
       </c>
-      <c r="E31" s="34"/>
-      <c r="F31" s="21" t="s">
+      <c r="E31" s="30"/>
+      <c r="F31" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="G31" s="57" t="s">
+      <c r="G31" s="46" t="s">
         <v>150</v>
       </c>
-      <c r="H31" s="58" t="s">
+      <c r="H31" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="I31" s="73" t="s">
+      <c r="I31" s="56" t="s">
         <v>151</v>
       </c>
-      <c r="J31" s="41"/>
-    </row>
-    <row r="32">
-      <c r="A32" s="15"/>
-      <c r="B32" s="31" t="s">
+      <c r="J31" s="26"/>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A32" s="11"/>
+      <c r="B32" s="27" t="s">
         <v>152</v>
       </c>
-      <c r="C32" s="32" t="s">
+      <c r="C32" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="D32" s="33" t="s">
+      <c r="D32" s="29" t="s">
         <v>153</v>
       </c>
-      <c r="E32" s="34"/>
-      <c r="G32" s="27"/>
-      <c r="H32" s="28"/>
-      <c r="I32" s="28"/>
-      <c r="J32" s="41"/>
-      <c r="L32" s="16" t="s">
+      <c r="E32" s="30"/>
+      <c r="G32" s="23"/>
+      <c r="H32" s="24"/>
+      <c r="I32" s="24"/>
+      <c r="J32" s="26"/>
+      <c r="L32" s="12" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A33" s="11"/>
+      <c r="B33" s="27" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="33">
-      <c r="A33" s="15"/>
-      <c r="B33" s="31" t="s">
+      <c r="C33" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="D33" s="29" t="s">
         <v>155</v>
       </c>
-      <c r="C33" s="32" t="s">
-        <v>37</v>
-      </c>
-      <c r="D33" s="33" t="s">
+      <c r="E33" s="30"/>
+      <c r="G33" s="23"/>
+      <c r="H33" s="24"/>
+      <c r="I33" s="24"/>
+      <c r="J33" s="30"/>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A34" s="6"/>
+      <c r="B34" s="27" t="s">
         <v>156</v>
       </c>
-      <c r="E33" s="34"/>
-      <c r="G33" s="39"/>
-      <c r="H33" s="74"/>
-      <c r="I33" s="74"/>
-      <c r="J33" s="34"/>
-    </row>
-    <row r="34">
-      <c r="A34" s="6"/>
-      <c r="B34" s="31" t="s">
+      <c r="C34" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="D34" s="29" t="s">
         <v>157</v>
       </c>
-      <c r="C34" s="32" t="s">
-        <v>72</v>
-      </c>
-      <c r="D34" s="33" t="s">
+      <c r="E34" s="30"/>
+      <c r="G34" s="23"/>
+      <c r="H34" s="24"/>
+      <c r="I34" s="24"/>
+      <c r="J34" s="30"/>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A35" s="11"/>
+      <c r="B35" s="27" t="s">
+        <v>80</v>
+      </c>
+      <c r="C35" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="D35" s="29" t="s">
         <v>158</v>
       </c>
-      <c r="E34" s="34"/>
-      <c r="G34" s="39"/>
-      <c r="H34" s="74"/>
-      <c r="I34" s="74"/>
-      <c r="J34" s="34"/>
-    </row>
-    <row r="35">
-      <c r="A35" s="15"/>
-      <c r="B35" s="31" t="s">
-        <v>80</v>
-      </c>
-      <c r="C35" s="32" t="s">
-        <v>4</v>
-      </c>
-      <c r="D35" s="33" t="s">
-        <v>159</v>
-      </c>
-      <c r="E35" s="34"/>
-      <c r="F35" s="15"/>
-      <c r="G35" s="75" t="s">
+      <c r="E35" s="30"/>
+      <c r="F35" s="11"/>
+      <c r="G35" s="57" t="s">
         <v>94</v>
       </c>
-      <c r="H35" s="39"/>
-      <c r="I35" s="74"/>
-      <c r="J35" s="76">
+      <c r="H35" s="23"/>
+      <c r="I35" s="24"/>
+      <c r="J35" s="58">
         <f>SUM(E4:E38,J4:J34)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="36">
-      <c r="A36" s="15"/>
-      <c r="B36" s="57" t="s">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A36" s="11"/>
+      <c r="B36" s="46" t="s">
+        <v>159</v>
+      </c>
+      <c r="C36" s="47" t="s">
+        <v>63</v>
+      </c>
+      <c r="D36" s="48" t="s">
         <v>160</v>
       </c>
-      <c r="C36" s="58" t="s">
-        <v>63</v>
-      </c>
-      <c r="D36" s="59" t="s">
+      <c r="E36" s="47"/>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A37" s="11"/>
+      <c r="B37" s="27" t="s">
         <v>161</v>
       </c>
-      <c r="E36" s="58"/>
-    </row>
-    <row r="37">
-      <c r="A37" s="15"/>
-      <c r="B37" s="31" t="s">
+      <c r="C37" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="D37" s="29" t="s">
         <v>162</v>
       </c>
-      <c r="C37" s="32" t="s">
-        <v>37</v>
-      </c>
-      <c r="D37" s="33" t="s">
+      <c r="E37" s="26"/>
+      <c r="F37" s="11"/>
+      <c r="G37" s="8"/>
+      <c r="H37" s="8"/>
+      <c r="I37" s="8"/>
+      <c r="J37" s="8"/>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A38" s="11"/>
+      <c r="B38" s="27" t="s">
         <v>163</v>
       </c>
-      <c r="E37" s="30"/>
-      <c r="F37" s="15"/>
-      <c r="G37" s="11"/>
-      <c r="H37" s="11"/>
-      <c r="I37" s="11"/>
-      <c r="J37" s="11"/>
-    </row>
-    <row r="38">
-      <c r="A38" s="15"/>
-      <c r="B38" s="31" t="s">
+      <c r="C38" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="D38" s="29" t="s">
         <v>164</v>
       </c>
-      <c r="C38" s="32" t="s">
-        <v>27</v>
-      </c>
-      <c r="D38" s="33" t="s">
-        <v>165</v>
-      </c>
-      <c r="E38" s="38"/>
-      <c r="G38" s="11"/>
-      <c r="H38" s="11"/>
-      <c r="I38" s="11"/>
-      <c r="J38" s="11"/>
-    </row>
-    <row r="39">
-      <c r="A39" s="15"/>
+      <c r="E38" s="30"/>
+      <c r="G38" s="8"/>
+      <c r="H38" s="8"/>
+      <c r="I38" s="8"/>
+      <c r="J38" s="8"/>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A39" s="11"/>
       <c r="G39" s="6"/>
       <c r="H39" s="6"/>
       <c r="I39" s="6"/>
-      <c r="J39" s="11"/>
-    </row>
-    <row r="40">
-      <c r="A40" s="15"/>
+      <c r="J39" s="8"/>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A40" s="11"/>
       <c r="G40" s="6"/>
       <c r="H40" s="6"/>
       <c r="I40" s="6"/>
-      <c r="J40" s="11"/>
-    </row>
-    <row r="41">
-      <c r="A41" s="15"/>
+      <c r="J40" s="8"/>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A41" s="11"/>
       <c r="B41" s="6"/>
       <c r="C41" s="6"/>
       <c r="D41" s="6"/>
       <c r="E41" s="6"/>
     </row>
-    <row r="42">
-      <c r="A42" s="15"/>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A42" s="11"/>
       <c r="B42" s="6"/>
       <c r="C42" s="6"/>
       <c r="D42" s="6"/>
       <c r="E42" s="6"/>
     </row>
-    <row r="43">
-      <c r="A43" s="15"/>
-      <c r="B43" s="11"/>
-      <c r="C43" s="11"/>
-      <c r="D43" s="11"/>
-      <c r="E43" s="11"/>
-    </row>
-    <row r="44">
-      <c r="A44" s="15"/>
-      <c r="B44" s="11"/>
-      <c r="C44" s="11"/>
-      <c r="D44" s="11"/>
-      <c r="E44" s="11"/>
-    </row>
-    <row r="45">
-      <c r="A45" s="15"/>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A43" s="11"/>
+      <c r="B43" s="8"/>
+      <c r="C43" s="8"/>
+      <c r="D43" s="8"/>
+      <c r="E43" s="8"/>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A44" s="11"/>
+      <c r="B44" s="8"/>
+      <c r="C44" s="8"/>
+      <c r="D44" s="8"/>
+      <c r="E44" s="8"/>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A45" s="11"/>
       <c r="E45" s="6"/>
     </row>
-    <row r="46">
-      <c r="A46" s="15"/>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A46" s="11"/>
       <c r="E46" s="6"/>
     </row>
-    <row r="47">
-      <c r="A47" s="15"/>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A47" s="11"/>
       <c r="E47" s="6"/>
-      <c r="F47" s="11"/>
-    </row>
-    <row r="48">
+      <c r="F47" s="8"/>
+    </row>
+    <row r="48" spans="1:15" ht="15" x14ac:dyDescent="0.2">
       <c r="A48" s="6"/>
-      <c r="E48" s="11"/>
-      <c r="F48" s="11"/>
-      <c r="L48" s="77"/>
-    </row>
-    <row r="49">
+      <c r="E48" s="8"/>
+      <c r="F48" s="8"/>
+      <c r="L48" s="63"/>
+      <c r="M48" s="64"/>
+      <c r="N48" s="64"/>
+      <c r="O48" s="64"/>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="6"/>
-      <c r="E49" s="11"/>
-      <c r="F49" s="15"/>
-      <c r="G49" s="11"/>
-      <c r="H49" s="11"/>
-      <c r="I49" s="11"/>
-      <c r="J49" s="11"/>
-      <c r="K49" s="77"/>
-    </row>
-    <row r="50">
+      <c r="E49" s="8"/>
+      <c r="F49" s="11"/>
+      <c r="G49" s="8"/>
+      <c r="H49" s="8"/>
+      <c r="I49" s="8"/>
+      <c r="J49" s="8"/>
+      <c r="K49" s="6"/>
+    </row>
+    <row r="50" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A50" s="6"/>
-      <c r="E50" s="11"/>
+      <c r="E50" s="8"/>
       <c r="F50" s="6"/>
       <c r="G50" s="6"/>
       <c r="H50" s="6"/>
       <c r="I50" s="6"/>
-      <c r="J50" s="11"/>
-    </row>
-    <row r="51">
+      <c r="J50" s="8"/>
+    </row>
+    <row r="51" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A51" s="6"/>
-      <c r="E51" s="11"/>
+      <c r="E51" s="8"/>
       <c r="G51" s="6"/>
       <c r="H51" s="6"/>
       <c r="I51" s="6"/>
-      <c r="J51" s="11"/>
-    </row>
-    <row r="52">
+      <c r="J51" s="8"/>
+    </row>
+    <row r="52" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A52" s="6"/>
-      <c r="E52" s="11"/>
-    </row>
-    <row r="53">
+      <c r="E52" s="8"/>
+    </row>
+    <row r="53" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A53" s="6"/>
-      <c r="E53" s="11"/>
-    </row>
-    <row r="54">
+      <c r="E53" s="8"/>
+    </row>
+    <row r="54" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A54" s="6"/>
-      <c r="E54" s="11"/>
-    </row>
-    <row r="55">
+      <c r="E54" s="8"/>
+    </row>
+    <row r="55" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A55" s="6"/>
-      <c r="E55" s="11"/>
-    </row>
-    <row r="56">
+      <c r="E55" s="8"/>
+    </row>
+    <row r="56" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A56" s="6"/>
       <c r="E56" s="6"/>
     </row>
-    <row r="57">
+    <row r="57" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A57" s="6"/>
       <c r="E57" s="6"/>
     </row>
-    <row r="58">
+    <row r="58" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A58" s="6"/>
     </row>
-    <row r="59">
+    <row r="59" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A59" s="6"/>
-      <c r="F59" s="11"/>
-    </row>
-    <row r="60">
-      <c r="A60" s="11"/>
+      <c r="F59" s="8"/>
+    </row>
+    <row r="60" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+      <c r="A60" s="8"/>
       <c r="F60" s="6"/>
     </row>
-    <row r="61">
-      <c r="A61" s="11"/>
+    <row r="61" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+      <c r="A61" s="8"/>
       <c r="F61" s="6"/>
     </row>
   </sheetData>
@@ -2284,9 +2237,8 @@
     <mergeCell ref="L23:P23"/>
     <mergeCell ref="L48:O48"/>
   </mergeCells>
-  <printOptions gridLines="1" horizontalCentered="1"/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup fitToHeight="0" cellComments="atEnd" orientation="portrait" pageOrder="overThenDown"/>
-  <drawing r:id="rId1"/>
+  <printOptions horizontalCentered="1" gridLines="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
+  <pageSetup fitToHeight="0" pageOrder="overThenDown" orientation="portrait" cellComments="atEnd"/>
 </worksheet>
 </file>
</xml_diff>